<commit_message>
modify feature likelihood charts
</commit_message>
<xml_diff>
--- a/writings/fig/1feature_lik.xlsx
+++ b/writings/fig/1feature_lik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhexuanxu/Documents/GitHub/hierarchical_bayesian/writings/fig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD80F117-80D0-C94F-BDB4-B3A14B8ADC8A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8E3A2985-2740-2647-BE5D-2968E3B6CDC1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38560" yWindow="460" windowWidth="37660" windowHeight="23540" xr2:uid="{89BF40B5-79FF-404F-8F6F-E8294ABD92B2}"/>
   </bookViews>
@@ -16,12 +16,6 @@
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">工作表1!$G$3:$G$62</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">工作表1!$H$3:$H$62</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">工作表1!$G$3:$G$62</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">工作表1!$H$3:$H$62</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -833,7 +827,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -846,14 +840,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2000" b="1"/>
               <a:t>P</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-Hans" sz="1600" b="1"/>
+              <a:rPr lang="en-US" altLang="zh-Hans" sz="2000" b="1"/>
               <a:t>OP</a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2000" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -870,7 +864,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1332,7 +1326,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1345,14 +1339,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-CN" sz="1200" b="1"/>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
                   <a:t>T</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1"/>
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1600" b="1"/>
                   <a:t>ime(Minutes)</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" b="1"/>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1369,7 +1363,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1455,7 +1449,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1468,10 +1462,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1200" b="1"/>
+                  <a:rPr lang="en-US" altLang="zh-Hans" sz="1600" b="1"/>
                   <a:t>Likelihood</a:t>
                 </a:r>
-                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1200" b="1"/>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1488,7 +1482,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -2779,6 +2773,62 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直线连接符 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{166B4748-2EB8-014D-B648-D4779BB00295}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4241800" y="1790700"/>
+          <a:ext cx="3238500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2786,12 +2836,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.34444</cdr:x>
-      <cdr:y>0.31019</cdr:y>
+      <cdr:x>0.36666</cdr:x>
+      <cdr:y>0.32408</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.36944</cdr:x>
-      <cdr:y>0.35185</cdr:y>
+      <cdr:x>0.39166</cdr:x>
+      <cdr:y>0.36574</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2806,8 +2856,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1574800" y="850900"/>
-          <a:ext cx="114300" cy="114300"/>
+          <a:off x="1676380" y="889013"/>
+          <a:ext cx="114300" cy="114282"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
           <a:avLst/>
@@ -3141,7 +3191,7 @@
   <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>